<commit_message>
Fixes to the data and addition of patch 7.1 data
</commit_message>
<xml_diff>
--- a/data/categories.xlsx
+++ b/data/categories.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="61">
   <si>
     <t>Category</t>
   </si>
@@ -85,6 +85,9 @@
     <t>Dragon</t>
   </si>
   <si>
+    <t>Demon</t>
+  </si>
+  <si>
     <t>Machine</t>
   </si>
   <si>
@@ -100,9 +103,6 @@
     <t>Elf</t>
   </si>
   <si>
-    <t>Demon</t>
-  </si>
-  <si>
     <t>Soldier</t>
   </si>
   <si>
@@ -130,15 +130,15 @@
     <t>Hazard</t>
   </si>
   <si>
+    <t>Wild Hunt</t>
+  </si>
+  <si>
     <t>Insectoid</t>
   </si>
   <si>
     <t>Necrophage</t>
   </si>
   <si>
-    <t>Wild Hunt</t>
-  </si>
-  <si>
     <t>Warrior</t>
   </si>
   <si>
@@ -160,6 +160,15 @@
     <t>Support</t>
   </si>
   <si>
+    <t>Pirate</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>card_category_74</t>
+  </si>
+  <si>
     <t>Warfare</t>
   </si>
   <si>
@@ -184,18 +193,18 @@
     <t>Druid</t>
   </si>
   <si>
-    <t>Pirate</t>
-  </si>
-  <si>
-    <t>Ship</t>
-  </si>
-  <si>
     <t>Raid</t>
   </si>
   <si>
     <t>Blindeyes</t>
   </si>
   <si>
+    <t>Salamandra</t>
+  </si>
+  <si>
+    <t>Firesworn</t>
+  </si>
+  <si>
     <t>Cutups</t>
   </si>
   <si>
@@ -205,16 +214,10 @@
     <t>Tidecloaks</t>
   </si>
   <si>
-    <t>Salamandra</t>
-  </si>
-  <si>
     <t>Cleric</t>
   </si>
   <si>
     <t>Witch Hunter</t>
-  </si>
-  <si>
-    <t>Firesworn</t>
   </si>
   <si>
     <t>Halfling</t>
@@ -600,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -644,7 +647,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -677,7 +680,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -688,7 +691,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -699,7 +702,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -726,18 +729,18 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -748,7 +751,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -759,7 +762,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -770,18 +773,18 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -852,7 +855,7 @@
         <v>27</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -937,7 +940,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -959,7 +962,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -970,7 +973,7 @@
         <v>20</v>
       </c>
       <c r="C3">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -981,7 +984,7 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -992,7 +995,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1003,7 +1006,7 @@
         <v>22</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1011,10 +1014,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1044,7 +1047,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -1063,10 +1066,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1074,10 +1077,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1099,9 +1102,64 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
     </row>
@@ -1131,10 +1189,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1238,7 +1296,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>44</v>
@@ -1249,7 +1307,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>22</v>
@@ -1260,10 +1318,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1274,7 +1332,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1282,29 +1340,29 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1312,21 +1370,21 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1334,10 +1392,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1348,7 +1406,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1391,10 +1449,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1445,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -1491,7 +1549,7 @@
         <v>23</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1599,7 +1657,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1610,26 +1668,26 @@
         <v>32</v>
       </c>
       <c r="C3">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>13</v>
@@ -1637,21 +1695,21 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -1659,21 +1717,21 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -1687,12 +1745,12 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1703,7 +1761,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -1714,7 +1772,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -1746,7 +1804,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -1757,13 +1815,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1848,7 +1906,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1856,7 +1914,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>14</v>
@@ -1864,21 +1922,21 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -1886,43 +1944,43 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -1930,10 +1988,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -1941,24 +1999,24 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1977,7 +2035,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -1988,7 +2046,7 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -1999,7 +2057,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -2007,10 +2065,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2018,10 +2076,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2032,7 +2090,7 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2043,7 +2101,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2108,29 +2166,29 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2138,10 +2196,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2149,10 +2207,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2163,7 +2221,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -2174,7 +2232,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2293,7 +2351,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2315,7 +2373,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2323,43 +2381,43 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2367,40 +2425,40 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -2408,43 +2466,43 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2452,13 +2510,13 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2477,7 +2535,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2485,10 +2543,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2496,12 +2554,23 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>1</v>
       </c>
     </row>
@@ -2512,7 +2581,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2539,12 +2608,23 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
@@ -2630,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2641,7 +2721,7 @@
         <v>20</v>
       </c>
       <c r="C3">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2652,7 +2732,7 @@
         <v>37</v>
       </c>
       <c r="C4">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2663,7 +2743,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2671,10 +2751,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2685,7 +2765,7 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2704,7 +2784,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -2715,7 +2795,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -2745,10 +2825,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2756,13 +2836,13 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>